<commit_message>
ANS-006-168 - Gestion des slices remontant un warning (#397)
* update binding VS

* update orga

* update Task VS

* ajout binding required

---------

Co-authored-by: TristanKereval <tristan.rieu@kereval.com> ea81bb05a781c89b957a3fbc68b9c7111704d01c
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-encounter-evenement.xlsx
+++ b/main/ig/StructureDefinition-tddui-encounter-evenement.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7095" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="848">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-17T14:24:53+00:00</t>
+    <t>2025-12-18T17:03:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1468,7 +1468,7 @@
     <t>Since there are many ways to further classify encounters, this element is 0..*.</t>
   </si>
   <si>
-    <t>https://hl7.fr/ig/fhir/core/ValueSet/fr-core-vs-encounter-type</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/tddui/ValueSet/tddui-encounter-type-vs</t>
   </si>
   <si>
     <t xml:space="preserve">pattern:coding.system}
@@ -1877,7 +1877,7 @@
     <t>The participant type indicates how an individual participates in an encounter. It includes non-practitioner participants, and for practitioners this is to describe the action type in the context of this encounter (e.g. Admitting Dr, Attending Dr, Translator, Consulting Dr). This is different to the practitioner roles which are functional roles, derived from terms of employment, education, licensing, etc.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/encounter-participant-type|4.0.1</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/tddui/ValueSet/tddui-encounter-participant-vs</t>
   </si>
   <si>
     <t>Event.performer.function</t>
@@ -12497,7 +12497,7 @@
         <v>82</v>
       </c>
       <c r="X82" t="s" s="2">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="Y82" s="2"/>
       <c r="Z82" t="s" s="2">
@@ -17877,11 +17877,9 @@
         <v>82</v>
       </c>
       <c r="X128" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="Y128" t="s" s="2">
-        <v>599</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y128" s="2"/>
       <c r="Z128" t="s" s="2">
         <v>601</v>
       </c>
@@ -18692,11 +18690,9 @@
         <v>82</v>
       </c>
       <c r="X135" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="Y135" t="s" s="2">
-        <v>599</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y135" s="2"/>
       <c r="Z135" t="s" s="2">
         <v>601</v>
       </c>
@@ -19507,11 +19503,9 @@
         <v>82</v>
       </c>
       <c r="X142" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="Y142" t="s" s="2">
-        <v>599</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y142" s="2"/>
       <c r="Z142" t="s" s="2">
         <v>601</v>
       </c>

</xml_diff>